<commit_message>
amino acid freq and synonomous codon dfs
</commit_message>
<xml_diff>
--- a/SynCodonsSGC.xlsx
+++ b/SynCodonsSGC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayrron Dale-Evans\python\code robustness\Code-robustness-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D2C83E-4E71-497D-8FF3-37CA917EFC9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38279CB1-DE50-4D91-BFD1-F24464C3CA67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{648ACA0A-F4C9-4F15-9739-B37883AF77E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{648ACA0A-F4C9-4F15-9739-B37883AF77E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Ala</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>n(a(c))</t>
+  </si>
+  <si>
+    <t>amino</t>
   </si>
 </sst>
 </file>
@@ -442,12 +445,15 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>

</xml_diff>